<commit_message>
gestionnaire emploi problème de cache du controlleur
</commit_message>
<xml_diff>
--- a/app/Fichiers Excel/Affectations.xlsx
+++ b/app/Fichiers Excel/Affectations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sora7\OneDrive\Desktop\PF SYN\eisgi_app\app\Fichiers Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8688D263-6479-4D4D-B0A4-BBFE0480096E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DA2308A-04A6-413A-9E73-402ABE57969F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{2D293D61-CA21-4919-9AD5-84B2F71E2DF7}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="123">
   <si>
     <t>anne de formation</t>
   </si>
@@ -411,10 +411,16 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -779,10 +785,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F71B7C9F-8F30-4001-9BF9-7442D59DC572}">
-  <dimension ref="A1:G35"/>
+  <dimension ref="A1:G36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:G1048576"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -841,22 +847,22 @@
         <v>7</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="C3" t="s">
-        <v>14</v>
+        <v>77</v>
       </c>
       <c r="D3" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="E3" t="s">
         <v>16</v>
       </c>
       <c r="F3" t="s">
-        <v>17</v>
+        <v>29</v>
       </c>
       <c r="G3" t="s">
-        <v>17</v>
+        <v>29</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
@@ -864,22 +870,22 @@
         <v>7</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="C4" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="D4" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="E4" t="s">
         <v>16</v>
       </c>
       <c r="F4" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="G4" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
@@ -887,22 +893,22 @@
         <v>7</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="C5" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="D5" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="E5" t="s">
         <v>16</v>
       </c>
       <c r="F5" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="G5" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
@@ -910,22 +916,22 @@
         <v>7</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="C6" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="D6" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="E6" t="s">
         <v>16</v>
       </c>
       <c r="F6" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="G6" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
@@ -933,22 +939,22 @@
         <v>7</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C7" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="D7" t="s">
-        <v>15</v>
+        <v>28</v>
       </c>
       <c r="E7" t="s">
-        <v>32</v>
+        <v>16</v>
       </c>
       <c r="F7" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="G7" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
@@ -956,22 +962,22 @@
         <v>7</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="C8" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="D8" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="E8" t="s">
         <v>32</v>
       </c>
       <c r="F8" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="G8" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
@@ -979,22 +985,22 @@
         <v>7</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C9" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="D9" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="E9" t="s">
         <v>32</v>
       </c>
       <c r="F9" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="G9" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
@@ -1002,22 +1008,22 @@
         <v>7</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C10" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="D10" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="E10" t="s">
         <v>32</v>
       </c>
       <c r="F10" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="G10" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
@@ -1025,22 +1031,22 @@
         <v>7</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C11" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="D11" t="s">
-        <v>45</v>
+        <v>28</v>
       </c>
       <c r="E11" t="s">
-        <v>11</v>
+        <v>32</v>
       </c>
       <c r="F11" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="G11" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
@@ -1048,22 +1054,22 @@
         <v>7</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="C12" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="D12" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="E12" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="F12" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="G12" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
@@ -1071,22 +1077,22 @@
         <v>7</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="C13" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="D13" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="E13" t="s">
         <v>16</v>
       </c>
       <c r="F13" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="G13" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
@@ -1094,22 +1100,22 @@
         <v>7</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="C14" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="D14" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="E14" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="F14" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="G14" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
@@ -1117,22 +1123,22 @@
         <v>7</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="C15" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="D15" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="E15" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="F15" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="G15" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
@@ -1140,22 +1146,22 @@
         <v>7</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="C16" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="D16" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="E16" t="s">
         <v>16</v>
       </c>
       <c r="F16" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="G16" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.3">
@@ -1163,22 +1169,22 @@
         <v>7</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="C17" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="D17" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="E17" t="s">
         <v>16</v>
       </c>
       <c r="F17" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="G17" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.3">
@@ -1186,22 +1192,22 @@
         <v>7</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="C18" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="D18" t="s">
-        <v>10</v>
+        <v>69</v>
       </c>
       <c r="E18" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="F18" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="G18" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.3">
@@ -1209,22 +1215,22 @@
         <v>7</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="C19" t="s">
-        <v>14</v>
+        <v>72</v>
       </c>
       <c r="D19" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="E19" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="F19" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="G19" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.3">
@@ -1232,22 +1238,22 @@
         <v>7</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C20" t="s">
-        <v>77</v>
+        <v>14</v>
       </c>
       <c r="D20" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="E20" t="s">
         <v>16</v>
       </c>
       <c r="F20" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="G20" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.3">
@@ -1255,22 +1261,22 @@
         <v>7</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="C21" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="D21" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="E21" t="s">
         <v>16</v>
       </c>
       <c r="F21" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="G21" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.3">
@@ -1278,22 +1284,22 @@
         <v>7</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="C22" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="D22" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="E22" t="s">
         <v>16</v>
       </c>
       <c r="F22" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="G22" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.3">
@@ -1301,22 +1307,22 @@
         <v>7</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="C23" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="D23" t="s">
-        <v>15</v>
+        <v>28</v>
       </c>
       <c r="E23" t="s">
-        <v>32</v>
+        <v>16</v>
       </c>
       <c r="F23" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="G23" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.3">
@@ -1324,22 +1330,22 @@
         <v>7</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="C24" t="s">
-        <v>35</v>
+        <v>86</v>
       </c>
       <c r="D24" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="E24" t="s">
         <v>32</v>
       </c>
       <c r="F24" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="G24" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.3">
@@ -1347,22 +1353,22 @@
         <v>7</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C25" t="s">
-        <v>91</v>
+        <v>35</v>
       </c>
       <c r="D25" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="E25" t="s">
         <v>32</v>
       </c>
       <c r="F25" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="G25" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.3">
@@ -1370,22 +1376,22 @@
         <v>7</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="C26" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="D26" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="E26" t="s">
         <v>32</v>
       </c>
       <c r="F26" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="G26" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.3">
@@ -1393,22 +1399,22 @@
         <v>7</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="C27" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="D27" t="s">
-        <v>45</v>
+        <v>28</v>
       </c>
       <c r="E27" t="s">
-        <v>11</v>
+        <v>32</v>
       </c>
       <c r="F27" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="G27" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.3">
@@ -1416,22 +1422,22 @@
         <v>7</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="C28" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="D28" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="E28" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="F28" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="G28" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.3">
@@ -1439,22 +1445,22 @@
         <v>7</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="C29" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="D29" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="E29" t="s">
         <v>16</v>
       </c>
       <c r="F29" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="G29" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.3">
@@ -1462,22 +1468,22 @@
         <v>7</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="C30" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="D30" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="E30" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="F30" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="G30" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.3">
@@ -1485,22 +1491,22 @@
         <v>7</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="C31" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="D31" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="E31" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="F31" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="G31" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.3">
@@ -1508,22 +1514,22 @@
         <v>7</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="C32" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="D32" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="E32" t="s">
         <v>16</v>
       </c>
       <c r="F32" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="G32" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.3">
@@ -1531,22 +1537,22 @@
         <v>7</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="C33" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="D33" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="E33" t="s">
         <v>16</v>
       </c>
       <c r="F33" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="G33" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.3">
@@ -1554,22 +1560,22 @@
         <v>7</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="C34" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="D34" t="s">
-        <v>10</v>
+        <v>69</v>
       </c>
       <c r="E34" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="F34" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="G34" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.3">
@@ -1577,25 +1583,49 @@
         <v>7</v>
       </c>
       <c r="B35" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="C35" t="s">
+        <v>118</v>
+      </c>
+      <c r="D35" t="s">
+        <v>10</v>
+      </c>
+      <c r="E35" t="s">
+        <v>11</v>
+      </c>
+      <c r="F35" t="s">
+        <v>119</v>
+      </c>
+      <c r="G35" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
+        <v>7</v>
+      </c>
+      <c r="B36" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="C35" t="s">
+      <c r="C36" t="s">
         <v>121</v>
       </c>
-      <c r="D35" t="s">
+      <c r="D36" t="s">
         <v>15</v>
       </c>
-      <c r="E35" t="s">
-        <v>16</v>
-      </c>
-      <c r="F35" t="s">
+      <c r="E36" t="s">
+        <v>16</v>
+      </c>
+      <c r="F36" t="s">
         <v>122</v>
       </c>
-      <c r="G35" t="s">
+      <c r="G36" t="s">
         <v>122</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>